<commit_message>
terminando traslados y calculo de depreciacion
</commit_message>
<xml_diff>
--- a/apps/empty_book.xlsx
+++ b/apps/empty_book.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:F6"/>
+  <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,63 +517,39 @@
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Para cubrir el incremento de la cartera </t>
+          <t>Osly Peralta</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Permanente</t>
+          <t>Temporal</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>Supervisor Legal</t>
+          <t>GESTOR DE COBROS</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>Julio</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr"/>
+          <t>Noviembre</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Diciembre</t>
+        </is>
+      </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>Para supervision a nivel nacional de los oficiales legales y abogados</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>Permanente</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>GESTOR DE COBROS DOMIC.</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>Enero</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr"/>
-      <c r="F6" s="3" t="inlineStr">
-        <is>
-          <t>asignado a la Regional Nor Occidente, ya que solo hay 1 gestor domiciliario y no se da abasto para cubrir la zona en vista que son 12 filiales</t>
+          <t>Cierre de año 2021</t>
         </is>
       </c>
     </row>

</xml_diff>